<commit_message>
Analytics work on sphere growth
</commit_message>
<xml_diff>
--- a/docs/out-data/TypeTrendlines.xlsx
+++ b/docs/out-data/TypeTrendlines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFEC89B-ACA1-3B4C-A5F2-933FCBBB3BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89072E12-D808-EE45-9595-07A130E2BC64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53540" yWindow="-28340" windowWidth="68800" windowHeight="28340" activeTab="4" xr2:uid="{B7C66097-5DE6-BF49-9D78-A6E5F57D9417}"/>
+    <workbookView xWindow="-53540" yWindow="-28340" windowWidth="68800" windowHeight="26740" activeTab="4" xr2:uid="{B7C66097-5DE6-BF49-9D78-A6E5F57D9417}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,13 @@
     <sheet name="Type8" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Type8!$F$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Type8!$F$2:$F$122</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Type8!$F$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Type8!$F$2:$F$122</definedName>
     <definedName name="nodes_count_cart_d_1" localSheetId="0">Type1!$A$1:$F$122</definedName>
     <definedName name="nodes_count_cart_d_105" localSheetId="4">Type8!$A$1:$F$122</definedName>
     <definedName name="nodes_count_cart_d_33" localSheetId="2">Type3!$A$1:$F$122</definedName>
     <definedName name="nodes_count_cart_d_57" localSheetId="3">Type4!$A$1:$F$122</definedName>
     <definedName name="nodes_count_cart_d_9" localSheetId="1">Type2!$A$1:$F$122</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +46,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{86AC6639-7C0B-1749-BBF9-34E1CB74162D}" name="nodes_count_cart_d_1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_1.csv" tab="0" comma="1">
+    <textPr sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_1.csv" tab="0" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -59,7 +55,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{F4CBBB77-9F65-6B48-9DEA-73F4513CAF6E}" name="nodes_count_cart_d_105" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_105.csv" tab="0" comma="1">
+    <textPr sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_105.csv" tab="0" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -68,7 +64,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{7F914F74-2D91-8345-A992-6CE07F996E61}" name="nodes_count_cart_d_33" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_33.csv" tab="0" comma="1">
+    <textPr sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_33.csv" tab="0" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -77,7 +73,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{23F5C29B-8E51-F44F-BEC9-C4475BE21F0A}" name="nodes_count_cart_d_57" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_57.csv" tab="0" comma="1">
+    <textPr sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_57.csv" tab="0" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -86,7 +82,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{365E7EB1-C0CA-774F-997F-50FBE7F380EC}" name="nodes_count_cart_d_9" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_9.csv" tab="0" comma="1">
+    <textPr sourceFile="/System/Volumes/Data/work/qsm/qsm-go/docs/out-data/nodes_count_cart_d_9.csv" tab="0" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -39062,7 +39058,7 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="0">A3-C3</f>
+        <f t="shared" ref="H3" si="0">A3-C3</f>
         <v>-0.41421356237310003</v>
       </c>
       <c r="I3">
@@ -42975,7 +42971,7 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="0">A3-C3</f>
+        <f t="shared" ref="H3" si="0">A3-C3</f>
         <v>-0.41421356237310003</v>
       </c>
       <c r="I3">
@@ -46888,7 +46884,7 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="0">A3-C3</f>
+        <f t="shared" ref="H3" si="0">A3-C3</f>
         <v>-0.41421356237310003</v>
       </c>
       <c r="I3">
@@ -50721,7 +50717,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12.1640625" customWidth="1"/>
   </cols>

</xml_diff>